<commit_message>
14th commit on 13-08-2019
</commit_message>
<xml_diff>
--- a/chemanalyst_14_07_2019/ChemAnalyst/MarketAnalysisImportfile/Demand by Grade(Tonnes).xlsx
+++ b/chemanalyst_14_07_2019/ChemAnalyst/MarketAnalysisImportfile/Demand by Grade(Tonnes).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Market Analysis Import Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Formats-05AUG\Market_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9930" windowHeight="4545"/>
+    <workbookView xWindow="4575" yWindow="1200" windowWidth="27645" windowHeight="15435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>